<commit_message>
docs: add closing process and final project report
</commit_message>
<xml_diff>
--- a/docs/resources/tables/cost-cumulative-report-2023-08-04.xlsx
+++ b/docs/resources/tables/cost-cumulative-report-2023-08-04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jahrim\Desktop\Projects\pm-project\docs\resources\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C37541C-8449-42F4-98BE-989F678F0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB0AF82-524C-4755-A241-85630250DEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Data
 Monitoraggio</t>
@@ -47,6 +47,17 @@
   </si>
   <si>
     <t>Stato progetto</t>
+  </si>
+  <si>
+    <t>Scadenza</t>
+  </si>
+  <si>
+    <t>Numero
+Scadenza</t>
+  </si>
+  <si>
+    <t>Linea
+Verticale</t>
   </si>
 </sst>
 </file>
@@ -90,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -209,12 +220,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -231,14 +282,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -292,7 +346,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cumulative Report - Schedule Trend</a:t>
+              <a:t>Cumulative Report - Cost Trend</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -350,6 +404,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Riserva di progetto</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -564,6 +621,164 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BCB7-4499-9F17-F992D8E4E457}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Scadenza</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-24D2-4EB1-9051-29930DC96B9A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.1146132242040311E-2"/>
+                  <c:y val="-5.1118219435690414E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="dd\-mm\-yyyy" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-24D2-4EB1-9051-29930DC96B9A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="dd\-mm\-yyyy" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>45152</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-50000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-24D2-4EB1-9051-29930DC96B9A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -711,6 +926,8 @@
         <c:axId val="622117999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50000"/>
+          <c:min val="-50000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -834,6 +1051,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34641579740313511"/>
+          <c:y val="5.9829615997855995E-2"/>
+          <c:w val="0.30716828413341091"/>
+          <c:h val="3.5942749606760353E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1429,16 +1687,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1381123</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1681</xdr:rowOff>
+      <xdr:rowOff>12887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>58830</xdr:rowOff>
+      <xdr:rowOff>70036</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1465,16 +1723,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>63203</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>184547</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>81131</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>142030</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>147633</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>79772</xdr:rowOff>
+      <xdr:rowOff>78442</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1489,8 +1747,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6194922" y="3625453"/>
-          <a:ext cx="7365452" cy="1419225"/>
+          <a:off x="10166425" y="3361765"/>
+          <a:ext cx="7327914" cy="1680883"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1648,12 +1906,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08371</cdr:x>
-      <cdr:y>0.0986</cdr:y>
+      <cdr:x>0.08378</cdr:x>
+      <cdr:y>0.09719</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.98249</cdr:x>
-      <cdr:y>0.41346</cdr:y>
+      <cdr:x>0.98256</cdr:x>
+      <cdr:y>0.38123</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1668,8 +1926,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="688103" y="587917"/>
-          <a:ext cx="7388040" cy="1877377"/>
+          <a:off x="683558" y="579513"/>
+          <a:ext cx="7333151" cy="1693600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1733,12 +1991,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08389</cdr:x>
-      <cdr:y>0.41346</cdr:y>
+      <cdr:x>0.08252</cdr:x>
+      <cdr:y>0.38151</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.98344</cdr:x>
-      <cdr:y>0.5748</cdr:y>
+      <cdr:x>0.98207</cdr:x>
+      <cdr:y>0.52781</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1753,8 +2011,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="690877" y="2465295"/>
-          <a:ext cx="7408257" cy="962024"/>
+          <a:off x="673253" y="2274817"/>
+          <a:ext cx="7339433" cy="872355"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2157,19 +2415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="20.7109375" customWidth="1"/>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2179,9 +2439,18 @@
       <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44981</v>
       </c>
@@ -2189,12 +2458,21 @@
         <f>A3</f>
         <v>44981</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>37500</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="E3" s="15">
+        <v>45152</v>
+      </c>
+      <c r="F3" s="16">
+        <f>E3</f>
+        <v>45152</v>
+      </c>
+      <c r="G3" s="13">
+        <v>50000</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3+7</f>
         <v>44988</v>
@@ -2203,12 +2481,21 @@
         <f>A4</f>
         <v>44988</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>33000</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="E4" s="17">
+        <v>45152</v>
+      </c>
+      <c r="F4" s="18">
+        <f>E4</f>
+        <v>45152</v>
+      </c>
+      <c r="G4" s="14">
+        <v>-50000</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A23" si="0">A4+7</f>
         <v>44995</v>
@@ -2217,12 +2504,11 @@
         <f t="shared" ref="B5:B26" si="1">A5</f>
         <v>44995</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>29500</v>
       </c>
-      <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45002</v>
@@ -2231,12 +2517,11 @@
         <f t="shared" si="1"/>
         <v>45002</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>15500</v>
       </c>
-      <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45009</v>
@@ -2245,12 +2530,11 @@
         <f t="shared" si="1"/>
         <v>45009</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>10000</v>
       </c>
-      <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45016</v>
@@ -2259,12 +2543,11 @@
         <f t="shared" si="1"/>
         <v>45016</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>5500</v>
       </c>
-      <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45023</v>
@@ -2273,12 +2556,11 @@
         <f t="shared" si="1"/>
         <v>45023</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>2000</v>
       </c>
-      <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>45030</v>
@@ -2287,12 +2569,11 @@
         <f t="shared" si="1"/>
         <v>45030</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>-15500</v>
       </c>
-      <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>45037</v>
@@ -2301,12 +2582,11 @@
         <f t="shared" si="1"/>
         <v>45037</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>22000</v>
       </c>
-      <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>45044</v>
@@ -2315,12 +2595,11 @@
         <f t="shared" si="1"/>
         <v>45044</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>19500</v>
       </c>
-      <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>45051</v>
@@ -2329,12 +2608,11 @@
         <f t="shared" si="1"/>
         <v>45051</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>15500</v>
       </c>
-      <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>45058</v>
@@ -2343,12 +2621,11 @@
         <f t="shared" si="1"/>
         <v>45058</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>3000</v>
       </c>
-      <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>45065</v>
@@ -2357,12 +2634,11 @@
         <f t="shared" si="1"/>
         <v>45065</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>500</v>
       </c>
-      <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>45072</v>
@@ -2371,12 +2647,11 @@
         <f t="shared" si="1"/>
         <v>45072</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>-2500</v>
       </c>
-      <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>45079</v>
@@ -2385,12 +2660,11 @@
         <f t="shared" si="1"/>
         <v>45079</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="12">
         <v>-7500</v>
       </c>
-      <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>45086</v>
@@ -2399,12 +2673,11 @@
         <f t="shared" si="1"/>
         <v>45086</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>-12000</v>
       </c>
-      <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>45093</v>
@@ -2413,12 +2686,11 @@
         <f t="shared" si="1"/>
         <v>45093</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <v>-27000</v>
       </c>
-      <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>45100</v>
@@ -2427,12 +2699,11 @@
         <f t="shared" si="1"/>
         <v>45100</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <v>12000</v>
       </c>
-      <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>45107</v>
@@ -2441,12 +2712,11 @@
         <f t="shared" si="1"/>
         <v>45107</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <v>8000</v>
       </c>
-      <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>45114</v>
@@ -2455,12 +2725,11 @@
         <f t="shared" si="1"/>
         <v>45114</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="12">
         <v>1000</v>
       </c>
-      <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>45121</v>
@@ -2469,11 +2738,11 @@
         <f t="shared" si="1"/>
         <v>45121</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="12">
         <v>-17000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f>A23+7</f>
         <v>45128</v>
@@ -2482,12 +2751,11 @@
         <f t="shared" si="1"/>
         <v>45128</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="12">
         <v>-24000</v>
       </c>
-      <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f>A24+7</f>
         <v>45135</v>
@@ -2496,12 +2764,11 @@
         <f t="shared" si="1"/>
         <v>45135</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="12">
         <v>-31000</v>
       </c>
-      <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f>A25+7</f>
         <v>45142</v>
@@ -2510,20 +2777,13 @@
         <f t="shared" si="1"/>
         <v>45142</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>32000</v>
       </c>
-      <c r="D26" s="10"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>